<commit_message>
Update Semaine 6/Journal de travail - Quentin Krenger.xlsx
quentin
</commit_message>
<xml_diff>
--- a/Semaine 6/Journal de travail - Quentin Krenger.xlsx
+++ b/Semaine 6/Journal de travail - Quentin Krenger.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD78CDE-A5FB-414B-A1BE-DF5D6EDF1A2E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>Tâche effectuées</t>
   </si>
@@ -123,13 +124,13 @@
     <t>Pas terminé</t>
   </si>
   <si>
-    <t>Date : 05.10.2018</t>
+    <t>Date : 04.11.2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -216,8 +217,12 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -225,15 +230,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -250,6 +248,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -344,6 +345,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -379,6 +397,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -554,14 +589,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B3:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45:G45"/>
+      <selection activeCell="B46" sqref="B46:E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,534 +606,517 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="3"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="6" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="2" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="3"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="3"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="6" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="3"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="6" t="s">
+      <c r="C13" s="2"/>
+      <c r="D13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="6" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="5"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="3"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="6" t="s">
+      <c r="C19" s="2"/>
+      <c r="D19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="5"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="3"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="5"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="6" t="s">
+      <c r="C21" s="2"/>
+      <c r="D21" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="5" t="s">
+      <c r="E21" s="3"/>
+      <c r="F21" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="3"/>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="3"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="5"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="6" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="5"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="3"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="5"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="6" t="s">
+      <c r="C26" s="2"/>
+      <c r="D26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="5"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="3"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="5"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="6" t="s">
+      <c r="C29" s="2"/>
+      <c r="D29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="5"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="3"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="5"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="6" t="s">
+      <c r="C32" s="2"/>
+      <c r="D32" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="5"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="3"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="5"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="6" t="s">
+      <c r="C35" s="2"/>
+      <c r="D35" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E35" s="6"/>
-      <c r="F35" s="5" t="s">
+      <c r="E35" s="3"/>
+      <c r="F35" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G35" s="3"/>
+      <c r="G35" s="5"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="3"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="5"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="6" t="s">
+      <c r="C38" s="2"/>
+      <c r="D38" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E38" s="6"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="5"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="3"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="5"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="6" t="s">
+      <c r="C40" s="2"/>
+      <c r="D40" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E40" s="6"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="5"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="3"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="5"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="6" t="s">
+      <c r="C43" s="2"/>
+      <c r="D43" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E43" s="6"/>
-      <c r="F43" s="2" t="s">
+      <c r="E43" s="3"/>
+      <c r="F43" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G43" s="3"/>
+      <c r="G43" s="5"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="3"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="5"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="3"/>
+      <c r="B46" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="5"/>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="3"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="5"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="3"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="5"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="3"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="5"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="3"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="5"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="3"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="B50:C51"/>
-    <mergeCell ref="D50:E51"/>
-    <mergeCell ref="F50:G51"/>
-    <mergeCell ref="B46:C47"/>
-    <mergeCell ref="D46:E47"/>
-    <mergeCell ref="F46:G47"/>
-    <mergeCell ref="B48:C49"/>
-    <mergeCell ref="D48:E49"/>
-    <mergeCell ref="F48:G49"/>
-    <mergeCell ref="B40:C41"/>
-    <mergeCell ref="D40:E41"/>
-    <mergeCell ref="F40:G41"/>
-    <mergeCell ref="B43:C44"/>
-    <mergeCell ref="D43:E44"/>
-    <mergeCell ref="F43:G44"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:C36"/>
-    <mergeCell ref="D35:E36"/>
-    <mergeCell ref="F35:G36"/>
-    <mergeCell ref="B38:C39"/>
-    <mergeCell ref="D38:E39"/>
-    <mergeCell ref="F38:G39"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="B6:C7"/>
-    <mergeCell ref="B8:C9"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="D8:E9"/>
-    <mergeCell ref="F6:G7"/>
-    <mergeCell ref="F8:G9"/>
-    <mergeCell ref="D13:E14"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="F29:G30"/>
+    <mergeCell ref="F32:G33"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="F11:G12"/>
+    <mergeCell ref="F13:G14"/>
+    <mergeCell ref="F16:G17"/>
+    <mergeCell ref="F19:G20"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="F24:G25"/>
+    <mergeCell ref="F26:G27"/>
+    <mergeCell ref="D26:E27"/>
+    <mergeCell ref="D29:E30"/>
+    <mergeCell ref="D32:E33"/>
+    <mergeCell ref="D11:E12"/>
+    <mergeCell ref="B29:C30"/>
     <mergeCell ref="B32:C33"/>
     <mergeCell ref="B11:C12"/>
     <mergeCell ref="B13:C14"/>
@@ -1115,22 +1133,43 @@
     <mergeCell ref="B26:C27"/>
     <mergeCell ref="B31:G31"/>
     <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="F29:G30"/>
-    <mergeCell ref="F32:G33"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="F11:G12"/>
-    <mergeCell ref="F13:G14"/>
-    <mergeCell ref="F16:G17"/>
-    <mergeCell ref="F19:G20"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="F24:G25"/>
-    <mergeCell ref="F26:G27"/>
-    <mergeCell ref="D26:E27"/>
-    <mergeCell ref="D29:E30"/>
-    <mergeCell ref="D32:E33"/>
-    <mergeCell ref="D11:E12"/>
-    <mergeCell ref="B29:C30"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="B8:C9"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="D8:E9"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="F8:G9"/>
+    <mergeCell ref="D13:E14"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:C36"/>
+    <mergeCell ref="D35:E36"/>
+    <mergeCell ref="F35:G36"/>
+    <mergeCell ref="B38:C39"/>
+    <mergeCell ref="D38:E39"/>
+    <mergeCell ref="F38:G39"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B40:C41"/>
+    <mergeCell ref="D40:E41"/>
+    <mergeCell ref="F40:G41"/>
+    <mergeCell ref="B43:C44"/>
+    <mergeCell ref="D43:E44"/>
+    <mergeCell ref="F43:G44"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="B50:C51"/>
+    <mergeCell ref="D50:E51"/>
+    <mergeCell ref="F50:G51"/>
+    <mergeCell ref="B46:C47"/>
+    <mergeCell ref="D46:E47"/>
+    <mergeCell ref="F46:G47"/>
+    <mergeCell ref="B48:C49"/>
+    <mergeCell ref="D48:E49"/>
+    <mergeCell ref="F48:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>